<commit_message>
refactored bracketCreate into 3 different components
</commit_message>
<xml_diff>
--- a/static/marchMadness/2026/results-bracket-march-madness-2026.xlsx
+++ b/static/marchMadness/2026/results-bracket-march-madness-2026.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E08A22B-B7C1-4FF9-BB20-A041A226C658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{8E08A22B-B7C1-4FF9-BB20-A041A226C658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5FFC0DB9-52FC-4332-8434-DEB4D2249312}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="89">
   <si>
     <t>2025 March Madness Bracket</t>
   </si>
@@ -660,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="I60" sqref="I60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1007,9 +1007,6 @@
       <c r="K30" t="s">
         <v>34</v>
       </c>
-      <c r="AD30" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="31" spans="2:39" x14ac:dyDescent="0.55000000000000004">
       <c r="B31">
@@ -1029,9 +1026,6 @@
       <c r="E32" t="s">
         <v>42</v>
       </c>
-      <c r="AJ32" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="33" spans="2:39" x14ac:dyDescent="0.55000000000000004">
       <c r="B33">
@@ -1051,9 +1045,6 @@
       <c r="H34" t="s">
         <v>42</v>
       </c>
-      <c r="AG34" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="35" spans="2:39" x14ac:dyDescent="0.55000000000000004">
       <c r="B35">
@@ -1101,9 +1092,6 @@
       <c r="O39" t="s">
         <v>15</v>
       </c>
-      <c r="W39" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="42" spans="2:39" x14ac:dyDescent="0.55000000000000004">
       <c r="B42">
@@ -1134,9 +1122,6 @@
       <c r="C44" t="s">
         <v>54</v>
       </c>
-      <c r="R44" t="s">
-        <v>15</v>
-      </c>
       <c r="AL44" t="s">
         <v>55</v>
       </c>
@@ -1195,9 +1180,6 @@
       <c r="K49" t="s">
         <v>52</v>
       </c>
-      <c r="AD49" t="s">
-        <v>53</v>
-      </c>
     </row>
     <row r="50" spans="2:39" x14ac:dyDescent="0.55000000000000004">
       <c r="B50">
@@ -1294,9 +1276,6 @@
       </c>
       <c r="N57" t="s">
         <v>52</v>
-      </c>
-      <c r="AA57" t="s">
-        <v>53</v>
       </c>
       <c r="AD57" t="s">
         <v>72</v>

</xml_diff>

<commit_message>
updated brackets display to show hypothetical winning scenarios
</commit_message>
<xml_diff>
--- a/static/marchMadness/2026/results-bracket-march-madness-2026.xlsx
+++ b/static/marchMadness/2026/results-bracket-march-madness-2026.xlsx
@@ -3,19 +3,32 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{8E08A22B-B7C1-4FF9-BB20-A041A226C658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5FFC0DB9-52FC-4332-8434-DEB4D2249312}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{8E08A22B-B7C1-4FF9-BB20-A041A226C658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27CE4800-EB76-4BAE-8A9D-683800B75C15}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="madness" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="87">
   <si>
     <t>2025 March Madness Bracket</t>
   </si>
@@ -158,13 +171,7 @@
     <t>Alabama</t>
   </si>
   <si>
-    <t>=O39</t>
-  </si>
-  <si>
     <t>Michigan St.</t>
-  </si>
-  <si>
-    <t>=W39</t>
   </si>
   <si>
     <t>Robert Morris</t>
@@ -334,6 +341,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -660,8 +671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="I60" sqref="I60"/>
+    <sheetView tabSelected="1" topLeftCell="G61" workbookViewId="0">
+      <selection activeCell="Q73" sqref="Q73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -825,9 +836,6 @@
       <c r="K14" t="s">
         <v>15</v>
       </c>
-      <c r="AD14" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="15" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="B15">
@@ -916,9 +924,6 @@
       <c r="N22" t="s">
         <v>15</v>
       </c>
-      <c r="AA22" t="s">
-        <v>16</v>
-      </c>
       <c r="AD22" t="s">
         <v>33</v>
       </c>
@@ -1053,11 +1058,8 @@
       <c r="C35" t="s">
         <v>46</v>
       </c>
-      <c r="T35" t="s">
+      <c r="AL35" t="s">
         <v>47</v>
-      </c>
-      <c r="AL35" t="s">
-        <v>48</v>
       </c>
       <c r="AM35">
         <v>2</v>
@@ -1067,11 +1069,8 @@
       <c r="E36" t="s">
         <v>46</v>
       </c>
-      <c r="T36" t="s">
-        <v>49</v>
-      </c>
       <c r="AJ36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="2:39" x14ac:dyDescent="0.55000000000000004">
@@ -1079,17 +1078,12 @@
         <v>15</v>
       </c>
       <c r="C37" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="AL37" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="AM37">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="39" spans="2:39" x14ac:dyDescent="0.55000000000000004">
-      <c r="O39" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1098,10 +1092,10 @@
         <v>1</v>
       </c>
       <c r="C42" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AL42" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="AM42">
         <v>1</v>
@@ -1109,10 +1103,10 @@
     </row>
     <row r="43" spans="2:39" x14ac:dyDescent="0.55000000000000004">
       <c r="E43" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AJ43" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="44" spans="2:39" x14ac:dyDescent="0.55000000000000004">
@@ -1120,10 +1114,10 @@
         <v>16</v>
       </c>
       <c r="C44" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AL44" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AM44">
         <v>16</v>
@@ -1131,10 +1125,10 @@
     </row>
     <row r="45" spans="2:39" x14ac:dyDescent="0.55000000000000004">
       <c r="H45" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AG45" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="46" spans="2:39" x14ac:dyDescent="0.55000000000000004">
@@ -1142,13 +1136,13 @@
         <v>8</v>
       </c>
       <c r="C46" t="s">
+        <v>54</v>
+      </c>
+      <c r="R46" t="s">
+        <v>55</v>
+      </c>
+      <c r="AL46" t="s">
         <v>56</v>
-      </c>
-      <c r="R46" t="s">
-        <v>57</v>
-      </c>
-      <c r="AL46" t="s">
-        <v>58</v>
       </c>
       <c r="AM46">
         <v>8</v>
@@ -1156,10 +1150,10 @@
     </row>
     <row r="47" spans="2:39" x14ac:dyDescent="0.55000000000000004">
       <c r="E47" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ47" t="s">
         <v>56</v>
-      </c>
-      <c r="AJ47" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="48" spans="2:39" x14ac:dyDescent="0.55000000000000004">
@@ -1167,18 +1161,13 @@
         <v>9</v>
       </c>
       <c r="C48" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AL48" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AM48">
         <v>9</v>
-      </c>
-    </row>
-    <row r="49" spans="2:39" x14ac:dyDescent="0.55000000000000004">
-      <c r="K49" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="50" spans="2:39" x14ac:dyDescent="0.55000000000000004">
@@ -1186,13 +1175,13 @@
         <v>5</v>
       </c>
       <c r="C50" t="s">
+        <v>59</v>
+      </c>
+      <c r="S50" t="s">
+        <v>60</v>
+      </c>
+      <c r="AL50" t="s">
         <v>61</v>
-      </c>
-      <c r="S50" t="s">
-        <v>62</v>
-      </c>
-      <c r="AL50" t="s">
-        <v>63</v>
       </c>
       <c r="AM50">
         <v>5</v>
@@ -1200,13 +1189,13 @@
     </row>
     <row r="51" spans="2:39" x14ac:dyDescent="0.55000000000000004">
       <c r="E51" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S51" t="s">
         <v>27</v>
       </c>
       <c r="AJ51" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="52" spans="2:39" x14ac:dyDescent="0.55000000000000004">
@@ -1214,10 +1203,10 @@
         <v>12</v>
       </c>
       <c r="C52" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="AL52" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="AM52">
         <v>12</v>
@@ -1225,10 +1214,10 @@
     </row>
     <row r="53" spans="2:39" x14ac:dyDescent="0.55000000000000004">
       <c r="H53" t="s">
+        <v>59</v>
+      </c>
+      <c r="AG53" t="s">
         <v>61</v>
-      </c>
-      <c r="AG53" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="54" spans="2:39" x14ac:dyDescent="0.55000000000000004">
@@ -1236,13 +1225,13 @@
         <v>4</v>
       </c>
       <c r="C54" t="s">
+        <v>64</v>
+      </c>
+      <c r="R54" t="s">
+        <v>65</v>
+      </c>
+      <c r="AL54" t="s">
         <v>66</v>
-      </c>
-      <c r="R54" t="s">
-        <v>67</v>
-      </c>
-      <c r="AL54" t="s">
-        <v>68</v>
       </c>
       <c r="AM54">
         <v>4</v>
@@ -1250,10 +1239,10 @@
     </row>
     <row r="55" spans="2:39" x14ac:dyDescent="0.55000000000000004">
       <c r="E55" t="s">
+        <v>64</v>
+      </c>
+      <c r="AJ55" t="s">
         <v>66</v>
-      </c>
-      <c r="AJ55" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="56" spans="2:39" x14ac:dyDescent="0.55000000000000004">
@@ -1261,10 +1250,10 @@
         <v>13</v>
       </c>
       <c r="C56" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="AL56" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AM56">
         <v>13</v>
@@ -1272,13 +1261,10 @@
     </row>
     <row r="57" spans="2:39" x14ac:dyDescent="0.55000000000000004">
       <c r="K57" t="s">
-        <v>71</v>
-      </c>
-      <c r="N57" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="AD57" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="58" spans="2:39" x14ac:dyDescent="0.55000000000000004">
@@ -1286,10 +1272,10 @@
         <v>6</v>
       </c>
       <c r="C58" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="AL58" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="AM58">
         <v>6</v>
@@ -1297,10 +1283,10 @@
     </row>
     <row r="59" spans="2:39" x14ac:dyDescent="0.55000000000000004">
       <c r="E59" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="AJ59" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="60" spans="2:39" x14ac:dyDescent="0.55000000000000004">
@@ -1308,10 +1294,10 @@
         <v>11</v>
       </c>
       <c r="C60" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="AL60" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="AM60">
         <v>11</v>
@@ -1319,10 +1305,10 @@
     </row>
     <row r="61" spans="2:39" x14ac:dyDescent="0.55000000000000004">
       <c r="H61" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="AG61" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="62" spans="2:39" x14ac:dyDescent="0.55000000000000004">
@@ -1330,10 +1316,10 @@
         <v>3</v>
       </c>
       <c r="C62" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AL62" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="AM62">
         <v>3</v>
@@ -1341,10 +1327,10 @@
     </row>
     <row r="63" spans="2:39" x14ac:dyDescent="0.55000000000000004">
       <c r="E63" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AJ63" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="64" spans="2:39" x14ac:dyDescent="0.55000000000000004">
@@ -1352,10 +1338,10 @@
         <v>14</v>
       </c>
       <c r="C64" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="AL64" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="AM64">
         <v>14</v>
@@ -1363,10 +1349,10 @@
     </row>
     <row r="65" spans="2:39" x14ac:dyDescent="0.55000000000000004">
       <c r="K65" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="AD65" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="66" spans="2:39" x14ac:dyDescent="0.55000000000000004">
@@ -1374,10 +1360,10 @@
         <v>7</v>
       </c>
       <c r="C66" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="AL66" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="AM66">
         <v>7</v>
@@ -1385,10 +1371,10 @@
     </row>
     <row r="67" spans="2:39" x14ac:dyDescent="0.55000000000000004">
       <c r="E67" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="AJ67" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="68" spans="2:39" x14ac:dyDescent="0.55000000000000004">
@@ -1396,10 +1382,10 @@
         <v>10</v>
       </c>
       <c r="C68" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="AL68" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="AM68">
         <v>10</v>
@@ -1407,10 +1393,10 @@
     </row>
     <row r="69" spans="2:39" x14ac:dyDescent="0.55000000000000004">
       <c r="H69" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="AG69" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="70" spans="2:39" x14ac:dyDescent="0.55000000000000004">
@@ -1418,10 +1404,10 @@
         <v>2</v>
       </c>
       <c r="C70" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="AL70" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="AM70">
         <v>2</v>
@@ -1429,10 +1415,10 @@
     </row>
     <row r="71" spans="2:39" x14ac:dyDescent="0.55000000000000004">
       <c r="E71" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="AJ71" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="72" spans="2:39" x14ac:dyDescent="0.55000000000000004">
@@ -1440,10 +1426,10 @@
         <v>15</v>
       </c>
       <c r="C72" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="AL72" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="AM72">
         <v>15</v>

</xml_diff>